<commit_message>
R script: all grouping done by unique_identifier
</commit_message>
<xml_diff>
--- a/alternative stimulus files/multiple IRAPs in a row/task.xlsx
+++ b/alternative stimulus files/multiple IRAPs in a row/task.xlsx
@@ -192,7 +192,8 @@
 Press either one to continue.</t>
   </si>
   <si>
-    <t>End of task 1. Take a short break.</t>
+    <t>End of task 1. Take a short break.
+Press the enter key to continue.</t>
   </si>
 </sst>
 </file>
@@ -1239,8 +1240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -1263,7 +1264,8 @@
     <col min="19" max="20" width="14.42578125" style="3" customWidth="1"/>
     <col min="21" max="22" width="20.7109375" style="3" customWidth="1"/>
     <col min="23" max="24" width="23.5703125" style="3" customWidth="1"/>
-    <col min="25" max="16384" width="10.7109375" style="3"/>
+    <col min="25" max="25" width="21.140625" style="3" customWidth="1"/>
+    <col min="26" max="16384" width="10.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25">
@@ -1369,7 +1371,7 @@
         <v>49</v>
       </c>
       <c r="I2" s="5">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J2" s="5">
         <v>2</v>
@@ -1396,7 +1398,7 @@
         <v>4</v>
       </c>
       <c r="R2" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>30</v>
@@ -1446,7 +1448,7 @@
         <v>47</v>
       </c>
       <c r="I3" s="5">
-        <v>0</v>
+        <v>80</v>
       </c>
       <c r="J3" s="5">
         <v>2</v>
@@ -1473,7 +1475,7 @@
         <v>4</v>
       </c>
       <c r="R3" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S3" s="3" t="s">
         <v>30</v>

</xml_diff>